<commit_message>
update model and feature
</commit_message>
<xml_diff>
--- a/ExportScoreData.xlsx
+++ b/ExportScoreData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhanga4\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codes\PythonCode\Solr_LTR\Solr_LTR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E35AD2CF-6004-4693-86A4-EF206FA61575}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114B36EB-9C0C-45DE-8D1E-DBB969C0BDF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <t>ScoreType</t>
   </si>
@@ -31,40 +31,10 @@
     <t>Score</t>
   </si>
   <si>
-    <t>個人情報</t>
-  </si>
-  <si>
-    <t>2212233217</t>
-  </si>
-  <si>
     <t>HUMAN_JUDGEMENT</t>
   </si>
   <si>
-    <t>2197372929</t>
-  </si>
-  <si>
-    <t>2212102145</t>
-  </si>
-  <si>
-    <t>2212036609</t>
-  </si>
-  <si>
-    <t>2197356545</t>
-  </si>
-  <si>
-    <t>2216771585</t>
-  </si>
-  <si>
-    <t>2212167681</t>
-  </si>
-  <si>
-    <t>2197274626</t>
-  </si>
-  <si>
-    <t>2197291010</t>
-  </si>
-  <si>
-    <t>2202746881</t>
+    <t>金融商品取引法</t>
   </si>
 </sst>
 </file>
@@ -72,13 +42,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="176" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -87,6 +57,19 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.3"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="SimSun"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,13 +92,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -431,20 +420,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="15" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="22" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -458,147 +447,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4">
+        <v>2441776051</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
+      <c r="B3" s="4">
+        <v>2342897476</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3309905217</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3309904961</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>